<commit_message>
Animated Plot/MTS Debug/Aug Lag Imp
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.1/Excel Files/flyball_governor.xlsx
+++ b/mbs-EP-v.1.0.1/Excel Files/flyball_governor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.1\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2CA3B3-A2F7-4F88-A0A4-ADD30FD3E34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73F2E07-BEE1-46E6-8A3D-86421981BE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="251">
   <si>
     <t>Mass</t>
   </si>
@@ -1953,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B2:Q39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="C3" s="84"/>
       <c r="D3" s="53">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E3" s="53" t="s">
         <v>22</v>
@@ -2373,7 +2373,9 @@
         <v>149</v>
       </c>
       <c r="C16" s="82"/>
-      <c r="D16" s="46"/>
+      <c r="D16" s="46" t="s">
+        <v>242</v>
+      </c>
       <c r="E16" s="50" t="s">
         <v>126</v>
       </c>
@@ -2905,7 +2907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AC35" sqref="AC35"/>
     </sheetView>
   </sheetViews>

</xml_diff>